<commit_message>
Modify humanland nad naturalland entity
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/人文景观.xlsx
+++ b/src/main/resources/xlsx/人文景观.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lichee\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lichee\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586A2DA6-1A43-4F55-B4E0-BE619CDA6E94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D07F85-B3D1-4A6D-A15A-79D5DAB82744}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3435" yWindow="420" windowWidth="17895" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据" sheetId="1" r:id="rId1"/>
@@ -52,13 +52,14 @@
     <t>文物保护单位</t>
   </si>
   <si>
-    <t>批准时间</t>
-  </si>
-  <si>
     <t>保护现状</t>
   </si>
   <si>
     <t>照片</t>
+  </si>
+  <si>
+    <t>原编号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -453,7 +454,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -493,13 +494,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>